<commit_message>
vg nav per share
</commit_message>
<xml_diff>
--- a/data/flow/EDV_fund_flow_data.xlsx
+++ b/data/flow/EDV_fund_flow_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B201"/>
+  <dimension ref="A1:B202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2445,6 +2445,16 @@
         <v>8.279999999999999</v>
       </c>
     </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2023-10-18</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
dump added main file
</commit_message>
<xml_diff>
--- a/data/flow/EDV_fund_flow_data.xlsx
+++ b/data/flow/EDV_fund_flow_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B202"/>
+  <dimension ref="A1:B203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2455,6 +2455,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2023-10-19</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>14.51475</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>